<commit_message>
Excercise 5 - fix
</commit_message>
<xml_diff>
--- a/00_homework_kawapa/Z5.xlsx
+++ b/00_homework_kawapa/Z5.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\multithreading\00_homework_kawapa\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="576" yWindow="72" windowWidth="22008" windowHeight="9504"/>
   </bookViews>
@@ -11,12 +16,12 @@
     <sheet name="Arkusz2" sheetId="2" r:id="rId2"/>
     <sheet name="Arkusz3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>Padding</t>
   </si>
@@ -38,12 +43,15 @@
   <si>
     <t>ms</t>
   </si>
+  <si>
+    <t>alignas(64)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,6 +72,12 @@
       <color theme="1"/>
       <name val="Czcionka tekstu podstawowego"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Czcionka tekstu podstawowego"/>
     </font>
   </fonts>
   <fills count="3">
@@ -350,7 +364,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -391,18 +405,37 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="pl-PL"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -415,18 +448,21 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Czas wykonania programu od wielkości "Padding"</a:t>
+              <a:t>Czas wykonania programu od wielkości "Padding" oraz stosując alignas(64)</a:t>
             </a:r>
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -490,6 +526,12 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6CE4-4DA7-ACD7-5CDDC4726B52}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -499,7 +541,7 @@
           </c:tx>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$C$20:$R$20</c:f>
+              <c:f>Arkusz1!$C$21:$R$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -554,9 +596,163 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6CE4-4DA7-ACD7-5CDDC4726B52}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
-        <c:dLbls/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>4 cores: alignas(64)</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz1!$C$11:$R$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>130.34200000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>146.91800000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>154.90799999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>152.405</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>158.423</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>157.41900000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>183.49199999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>190.999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>198.52600000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>176.971</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>206.05799999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>182.98</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>188.00200000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>186.99799999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>177.46799999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>174.96600000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-6CE4-4DA7-ACD7-5CDDC4726B52}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>2 cores: alignas(64)</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz1!$C$22:$R$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>82.679000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>89.275499999999994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>91.245599999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>83.225099999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>84.73</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>112.809</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>113.81</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>113.301</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>124.33199999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>117.312</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>98.2607</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>79.713499999999996</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>81.215199999999996</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>95.755099999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>80.217600000000004</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>78.213399999999993</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-6CE4-4DA7-ACD7-5CDDC4726B52}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
+        <c:smooth val="0"/>
         <c:axId val="205039104"/>
         <c:axId val="205041024"/>
       </c:lineChart>
@@ -565,20 +761,24 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="205041024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="205041024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -599,9 +799,11 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="205039104"/>
         <c:crosses val="autoZero"/>
@@ -611,8 +813,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -627,15 +832,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>508362</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>18506</xdr:rowOff>
+      <xdr:colOff>388619</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>73256</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>163286</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>628427</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>130629</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -658,9 +863,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -698,9 +903,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -732,9 +937,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -766,9 +972,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -941,11 +1148,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:S23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:S24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S17" sqref="S17:T17"/>
+      <selection activeCell="Y11" sqref="Y11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1329,7 +1536,7 @@
         <v>717.38779999999997</v>
       </c>
       <c r="E10" s="10">
-        <f t="shared" ref="D10:S10" si="0">AVERAGE(E5:E9)</f>
+        <f t="shared" ref="E10:R10" si="0">AVERAGE(E5:E9)</f>
         <v>840.38279999999997</v>
       </c>
       <c r="F10" s="10">
@@ -1388,493 +1595,547 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="2:19" ht="14.4" thickBot="1">
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
+    <row r="11" spans="2:19">
+      <c r="B11" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1">
+        <v>130.34200000000001</v>
+      </c>
+      <c r="D11" s="1">
+        <v>146.91800000000001</v>
+      </c>
+      <c r="E11" s="1">
+        <v>154.90799999999999</v>
+      </c>
+      <c r="F11" s="1">
+        <v>152.405</v>
+      </c>
+      <c r="G11" s="1">
+        <v>158.423</v>
+      </c>
+      <c r="H11" s="1">
+        <v>157.41900000000001</v>
+      </c>
+      <c r="I11" s="1">
+        <v>183.49199999999999</v>
+      </c>
+      <c r="J11" s="1">
+        <v>190.999</v>
+      </c>
+      <c r="K11" s="1">
+        <v>198.52600000000001</v>
+      </c>
+      <c r="L11" s="1">
+        <v>176.971</v>
+      </c>
+      <c r="M11" s="1">
+        <v>206.05799999999999</v>
+      </c>
+      <c r="N11" s="1">
+        <v>182.98</v>
+      </c>
+      <c r="O11" s="1">
+        <v>188.00200000000001</v>
+      </c>
+      <c r="P11" s="1">
+        <v>186.99799999999999</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>177.46799999999999</v>
+      </c>
+      <c r="R11" s="1">
+        <v>174.96600000000001</v>
+      </c>
       <c r="S11" s="2"/>
     </row>
-    <row r="12" spans="2:19">
-      <c r="B12" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="5"/>
+    <row r="12" spans="2:19" ht="14.4" thickBot="1">
       <c r="S12" s="2"/>
     </row>
-    <row r="13" spans="2:19" ht="14.4" thickBot="1">
-      <c r="B13" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="13"/>
-      <c r="R13" s="14"/>
+    <row r="13" spans="2:19">
+      <c r="B13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="5"/>
       <c r="S13" s="2"/>
     </row>
     <row r="14" spans="2:19" ht="14.4" thickBot="1">
-      <c r="B14" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="19">
-        <v>0</v>
-      </c>
-      <c r="D14" s="19">
-        <v>1</v>
-      </c>
-      <c r="E14" s="19">
+      <c r="B14" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F14" s="19">
-        <v>3</v>
-      </c>
-      <c r="G14" s="19">
-        <v>4</v>
-      </c>
-      <c r="H14" s="19">
-        <v>5</v>
-      </c>
-      <c r="I14" s="19">
-        <v>6</v>
-      </c>
-      <c r="J14" s="19">
-        <v>7</v>
-      </c>
-      <c r="K14" s="19">
-        <v>8</v>
-      </c>
-      <c r="L14" s="19">
-        <v>9</v>
-      </c>
-      <c r="M14" s="19">
-        <v>10</v>
-      </c>
-      <c r="N14" s="19">
-        <v>11</v>
-      </c>
-      <c r="O14" s="19">
-        <v>12</v>
-      </c>
-      <c r="P14" s="19">
-        <v>13</v>
-      </c>
-      <c r="Q14" s="19">
-        <v>14</v>
-      </c>
-      <c r="R14" s="20">
-        <v>15</v>
-      </c>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="14"/>
       <c r="S14" s="2"/>
     </row>
-    <row r="15" spans="2:19">
-      <c r="B15" s="15"/>
-      <c r="C15" s="16">
-        <v>653.26099999999997</v>
-      </c>
-      <c r="D15" s="16">
-        <v>518.005</v>
-      </c>
-      <c r="E15" s="16">
-        <v>712.83900000000006</v>
-      </c>
-      <c r="F15" s="16">
-        <v>582.56399999999996</v>
-      </c>
-      <c r="G15" s="16">
-        <v>584.13499999999999</v>
-      </c>
-      <c r="H15" s="16">
-        <v>702.39499999999998</v>
-      </c>
-      <c r="I15" s="16">
-        <v>629.51400000000001</v>
-      </c>
-      <c r="J15" s="16">
-        <v>756.404</v>
-      </c>
-      <c r="K15" s="16">
-        <v>745.399</v>
-      </c>
-      <c r="L15" s="16">
-        <v>134.798</v>
-      </c>
-      <c r="M15" s="16">
-        <v>127.03400000000001</v>
-      </c>
-      <c r="N15" s="16">
-        <v>125.488</v>
-      </c>
-      <c r="O15" s="16">
-        <v>121.029</v>
-      </c>
-      <c r="P15" s="16">
-        <v>129.035</v>
-      </c>
-      <c r="Q15" s="16">
-        <v>130.03</v>
-      </c>
-      <c r="R15" s="17">
-        <v>142.35599999999999</v>
+    <row r="15" spans="2:19" ht="14.4" thickBot="1">
+      <c r="B15" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="19">
+        <v>0</v>
+      </c>
+      <c r="D15" s="19">
+        <v>1</v>
+      </c>
+      <c r="E15" s="19">
+        <v>2</v>
+      </c>
+      <c r="F15" s="19">
+        <v>3</v>
+      </c>
+      <c r="G15" s="19">
+        <v>4</v>
+      </c>
+      <c r="H15" s="19">
+        <v>5</v>
+      </c>
+      <c r="I15" s="19">
+        <v>6</v>
+      </c>
+      <c r="J15" s="19">
+        <v>7</v>
+      </c>
+      <c r="K15" s="19">
+        <v>8</v>
+      </c>
+      <c r="L15" s="19">
+        <v>9</v>
+      </c>
+      <c r="M15" s="19">
+        <v>10</v>
+      </c>
+      <c r="N15" s="19">
+        <v>11</v>
+      </c>
+      <c r="O15" s="19">
+        <v>12</v>
+      </c>
+      <c r="P15" s="19">
+        <v>13</v>
+      </c>
+      <c r="Q15" s="19">
+        <v>14</v>
+      </c>
+      <c r="R15" s="20">
+        <v>15</v>
       </c>
       <c r="S15" s="2"/>
     </row>
     <row r="16" spans="2:19">
-      <c r="B16" s="6"/>
-      <c r="C16" s="7">
-        <v>484.03899999999999</v>
-      </c>
-      <c r="D16" s="7">
-        <v>404.22899999999998</v>
-      </c>
-      <c r="E16" s="7">
-        <v>621.99900000000002</v>
-      </c>
-      <c r="F16" s="7">
-        <v>586.71</v>
-      </c>
-      <c r="G16" s="7">
-        <v>544.04</v>
-      </c>
-      <c r="H16" s="7">
-        <v>703.89800000000002</v>
-      </c>
-      <c r="I16" s="7">
-        <v>870.38099999999997</v>
-      </c>
-      <c r="J16" s="7">
-        <v>639.29200000000003</v>
-      </c>
-      <c r="K16" s="7">
-        <v>651.81100000000004</v>
-      </c>
-      <c r="L16" s="7">
-        <v>143</v>
-      </c>
-      <c r="M16" s="7">
-        <v>150.114</v>
-      </c>
-      <c r="N16" s="7">
-        <v>145.56</v>
-      </c>
-      <c r="O16" s="7">
-        <v>137.059</v>
-      </c>
-      <c r="P16" s="7">
-        <v>143.471</v>
-      </c>
-      <c r="Q16" s="7">
-        <v>136.13399999999999</v>
-      </c>
-      <c r="R16" s="8">
-        <v>149.88800000000001</v>
+      <c r="B16" s="15"/>
+      <c r="C16" s="16">
+        <v>653.26099999999997</v>
+      </c>
+      <c r="D16" s="16">
+        <v>518.005</v>
+      </c>
+      <c r="E16" s="16">
+        <v>712.83900000000006</v>
+      </c>
+      <c r="F16" s="16">
+        <v>582.56399999999996</v>
+      </c>
+      <c r="G16" s="16">
+        <v>584.13499999999999</v>
+      </c>
+      <c r="H16" s="16">
+        <v>702.39499999999998</v>
+      </c>
+      <c r="I16" s="16">
+        <v>629.51400000000001</v>
+      </c>
+      <c r="J16" s="16">
+        <v>756.404</v>
+      </c>
+      <c r="K16" s="16">
+        <v>745.399</v>
+      </c>
+      <c r="L16" s="16">
+        <v>134.798</v>
+      </c>
+      <c r="M16" s="16">
+        <v>127.03400000000001</v>
+      </c>
+      <c r="N16" s="16">
+        <v>125.488</v>
+      </c>
+      <c r="O16" s="16">
+        <v>121.029</v>
+      </c>
+      <c r="P16" s="16">
+        <v>129.035</v>
+      </c>
+      <c r="Q16" s="16">
+        <v>130.03</v>
+      </c>
+      <c r="R16" s="17">
+        <v>142.35599999999999</v>
       </c>
       <c r="S16" s="2"/>
     </row>
     <row r="17" spans="2:19">
       <c r="B17" s="6"/>
       <c r="C17" s="7">
-        <v>772.005</v>
+        <v>484.03899999999999</v>
       </c>
       <c r="D17" s="7">
-        <v>609.50699999999995</v>
+        <v>404.22899999999998</v>
       </c>
       <c r="E17" s="7">
-        <v>779.34</v>
+        <v>621.99900000000002</v>
       </c>
       <c r="F17" s="7">
-        <v>684.09299999999996</v>
+        <v>586.71</v>
       </c>
       <c r="G17" s="7">
-        <v>537.12199999999996</v>
+        <v>544.04</v>
       </c>
       <c r="H17" s="7">
-        <v>592.995</v>
+        <v>703.89800000000002</v>
       </c>
       <c r="I17" s="7">
-        <v>564.44500000000005</v>
+        <v>870.38099999999997</v>
       </c>
       <c r="J17" s="7">
-        <v>550.005</v>
+        <v>639.29200000000003</v>
       </c>
       <c r="K17" s="7">
-        <v>628.995</v>
+        <v>651.81100000000004</v>
       </c>
       <c r="L17" s="7">
-        <v>135.005</v>
+        <v>143</v>
       </c>
       <c r="M17" s="7">
-        <v>139.17599999999999</v>
+        <v>150.114</v>
       </c>
       <c r="N17" s="7">
-        <v>133.36099999999999</v>
+        <v>145.56</v>
       </c>
       <c r="O17" s="7">
-        <v>133.03100000000001</v>
+        <v>137.059</v>
       </c>
       <c r="P17" s="7">
-        <v>147.48400000000001</v>
+        <v>143.471</v>
       </c>
       <c r="Q17" s="7">
-        <v>133.05099999999999</v>
+        <v>136.13399999999999</v>
       </c>
       <c r="R17" s="8">
-        <v>127.017</v>
+        <v>149.88800000000001</v>
       </c>
       <c r="S17" s="2"/>
     </row>
     <row r="18" spans="2:19">
       <c r="B18" s="6"/>
       <c r="C18" s="7">
-        <v>933.005</v>
+        <v>772.005</v>
       </c>
       <c r="D18" s="7">
-        <v>613.99400000000003</v>
+        <v>609.50699999999995</v>
       </c>
       <c r="E18" s="7">
-        <v>673.23199999999997</v>
+        <v>779.34</v>
       </c>
       <c r="F18" s="7">
-        <v>704.19399999999996</v>
+        <v>684.09299999999996</v>
       </c>
       <c r="G18" s="7">
-        <v>574.99300000000005</v>
+        <v>537.12199999999996</v>
       </c>
       <c r="H18" s="7">
-        <v>732.17</v>
+        <v>592.995</v>
       </c>
       <c r="I18" s="7">
-        <v>568.005</v>
+        <v>564.44500000000005</v>
       </c>
       <c r="J18" s="7">
-        <v>539.68399999999997</v>
+        <v>550.005</v>
       </c>
       <c r="K18" s="7">
-        <v>597.048</v>
+        <v>628.995</v>
       </c>
       <c r="L18" s="7">
-        <v>135.999</v>
+        <v>135.005</v>
       </c>
       <c r="M18" s="7">
-        <v>133.74600000000001</v>
+        <v>139.17599999999999</v>
       </c>
       <c r="N18" s="7">
-        <v>133.81399999999999</v>
+        <v>133.36099999999999</v>
       </c>
       <c r="O18" s="7">
-        <v>137.602</v>
+        <v>133.03100000000001</v>
       </c>
       <c r="P18" s="7">
-        <v>148.73400000000001</v>
+        <v>147.48400000000001</v>
       </c>
       <c r="Q18" s="7">
-        <v>134.786</v>
+        <v>133.05099999999999</v>
       </c>
       <c r="R18" s="8">
-        <v>133.03899999999999</v>
+        <v>127.017</v>
       </c>
       <c r="S18" s="2"/>
     </row>
     <row r="19" spans="2:19">
       <c r="B19" s="6"/>
       <c r="C19" s="7">
-        <v>768.74400000000003</v>
+        <v>933.005</v>
       </c>
       <c r="D19" s="7">
-        <v>815.53800000000001</v>
+        <v>613.99400000000003</v>
       </c>
       <c r="E19" s="7">
-        <v>865.64099999999996</v>
+        <v>673.23199999999997</v>
       </c>
       <c r="F19" s="7">
-        <v>926.14</v>
+        <v>704.19399999999996</v>
       </c>
       <c r="G19" s="7">
-        <v>802.50900000000001</v>
+        <v>574.99300000000005</v>
       </c>
       <c r="H19" s="7">
-        <v>593.61599999999999</v>
+        <v>732.17</v>
       </c>
       <c r="I19" s="7">
-        <v>623.50800000000004</v>
+        <v>568.005</v>
       </c>
       <c r="J19" s="7">
-        <v>687.452</v>
+        <v>539.68399999999997</v>
       </c>
       <c r="K19" s="7">
-        <v>869.625</v>
+        <v>597.048</v>
       </c>
       <c r="L19" s="7">
-        <v>136</v>
+        <v>135.999</v>
       </c>
       <c r="M19" s="7">
-        <v>161.916</v>
+        <v>133.74600000000001</v>
       </c>
       <c r="N19" s="7">
-        <v>133.21</v>
+        <v>133.81399999999999</v>
       </c>
       <c r="O19" s="7">
-        <v>138</v>
+        <v>137.602</v>
       </c>
       <c r="P19" s="7">
-        <v>138.053</v>
+        <v>148.73400000000001</v>
       </c>
       <c r="Q19" s="7">
-        <v>142.71899999999999</v>
+        <v>134.786</v>
       </c>
       <c r="R19" s="8">
-        <v>131.00700000000001</v>
+        <v>133.03899999999999</v>
       </c>
       <c r="S19" s="2"/>
     </row>
-    <row r="20" spans="2:19" ht="14.4" thickBot="1">
-      <c r="B20" s="9" t="s">
+    <row r="20" spans="2:19">
+      <c r="B20" s="6"/>
+      <c r="C20" s="7">
+        <v>768.74400000000003</v>
+      </c>
+      <c r="D20" s="7">
+        <v>815.53800000000001</v>
+      </c>
+      <c r="E20" s="7">
+        <v>865.64099999999996</v>
+      </c>
+      <c r="F20" s="7">
+        <v>926.14</v>
+      </c>
+      <c r="G20" s="7">
+        <v>802.50900000000001</v>
+      </c>
+      <c r="H20" s="7">
+        <v>593.61599999999999</v>
+      </c>
+      <c r="I20" s="7">
+        <v>623.50800000000004</v>
+      </c>
+      <c r="J20" s="7">
+        <v>687.452</v>
+      </c>
+      <c r="K20" s="7">
+        <v>869.625</v>
+      </c>
+      <c r="L20" s="7">
+        <v>136</v>
+      </c>
+      <c r="M20" s="7">
+        <v>161.916</v>
+      </c>
+      <c r="N20" s="7">
+        <v>133.21</v>
+      </c>
+      <c r="O20" s="7">
+        <v>138</v>
+      </c>
+      <c r="P20" s="7">
+        <v>138.053</v>
+      </c>
+      <c r="Q20" s="7">
+        <v>142.71899999999999</v>
+      </c>
+      <c r="R20" s="8">
+        <v>131.00700000000001</v>
+      </c>
+      <c r="S20" s="2"/>
+    </row>
+    <row r="21" spans="2:19" ht="14.4" thickBot="1">
+      <c r="B21" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="10">
-        <f>AVERAGE(C15:C19)</f>
+      <c r="C21" s="10">
+        <f>AVERAGE(C16:C20)</f>
         <v>722.21080000000006</v>
       </c>
-      <c r="D20" s="10">
-        <f>AVERAGE(D15:D19)</f>
+      <c r="D21" s="10">
+        <f>AVERAGE(D16:D20)</f>
         <v>592.25459999999998</v>
       </c>
-      <c r="E20" s="10">
-        <f t="shared" ref="E20" si="1">AVERAGE(E15:E19)</f>
+      <c r="E21" s="10">
+        <f t="shared" ref="E21" si="1">AVERAGE(E16:E20)</f>
         <v>730.61020000000008</v>
       </c>
-      <c r="F20" s="10">
-        <f t="shared" ref="F20" si="2">AVERAGE(F15:F19)</f>
+      <c r="F21" s="10">
+        <f t="shared" ref="F21" si="2">AVERAGE(F16:F20)</f>
         <v>696.74019999999996</v>
       </c>
-      <c r="G20" s="10">
-        <f>AVERAGE(G15:G19)</f>
+      <c r="G21" s="10">
+        <f>AVERAGE(G16:G20)</f>
         <v>608.5598</v>
       </c>
-      <c r="H20" s="10">
-        <f t="shared" ref="H20" si="3">AVERAGE(H15:H19)</f>
+      <c r="H21" s="10">
+        <f t="shared" ref="H21" si="3">AVERAGE(H16:H20)</f>
         <v>665.01480000000004</v>
       </c>
-      <c r="I20" s="10">
-        <f t="shared" ref="I20" si="4">AVERAGE(I15:I19)</f>
+      <c r="I21" s="10">
+        <f t="shared" ref="I21" si="4">AVERAGE(I16:I20)</f>
         <v>651.17060000000004</v>
       </c>
-      <c r="J20" s="10">
-        <f t="shared" ref="J20" si="5">AVERAGE(J15:J19)</f>
+      <c r="J21" s="10">
+        <f t="shared" ref="J21" si="5">AVERAGE(J16:J20)</f>
         <v>634.56740000000013</v>
       </c>
-      <c r="K20" s="10">
-        <f t="shared" ref="K20" si="6">AVERAGE(K15:K19)</f>
+      <c r="K21" s="10">
+        <f t="shared" ref="K21" si="6">AVERAGE(K16:K20)</f>
         <v>698.57559999999989</v>
       </c>
-      <c r="L20" s="10">
-        <f t="shared" ref="L20" si="7">AVERAGE(L15:L19)</f>
+      <c r="L21" s="10">
+        <f t="shared" ref="L21" si="7">AVERAGE(L16:L20)</f>
         <v>136.96039999999999</v>
       </c>
-      <c r="M20" s="10">
-        <f t="shared" ref="M20" si="8">AVERAGE(M15:M19)</f>
+      <c r="M21" s="10">
+        <f t="shared" ref="M21" si="8">AVERAGE(M16:M20)</f>
         <v>142.39720000000003</v>
       </c>
-      <c r="N20" s="10">
-        <f t="shared" ref="N20" si="9">AVERAGE(N15:N19)</f>
+      <c r="N21" s="10">
+        <f t="shared" ref="N21" si="9">AVERAGE(N16:N20)</f>
         <v>134.28659999999999</v>
       </c>
-      <c r="O20" s="10">
-        <f t="shared" ref="O20" si="10">AVERAGE(O15:O19)</f>
+      <c r="O21" s="10">
+        <f t="shared" ref="O21" si="10">AVERAGE(O16:O20)</f>
         <v>133.3442</v>
       </c>
-      <c r="P20" s="10">
-        <f t="shared" ref="P20" si="11">AVERAGE(P15:P19)</f>
+      <c r="P21" s="10">
+        <f t="shared" ref="P21" si="11">AVERAGE(P16:P20)</f>
         <v>141.3554</v>
       </c>
-      <c r="Q20" s="10">
-        <f t="shared" ref="Q20" si="12">AVERAGE(Q15:Q19)</f>
+      <c r="Q21" s="10">
+        <f t="shared" ref="Q21" si="12">AVERAGE(Q16:Q20)</f>
         <v>135.34399999999999</v>
       </c>
-      <c r="R20" s="11">
-        <f t="shared" ref="R20" si="13">AVERAGE(R15:R19)</f>
+      <c r="R21" s="11">
+        <f t="shared" ref="R21" si="13">AVERAGE(R16:R20)</f>
         <v>136.66140000000001</v>
       </c>
-      <c r="S20" s="2" t="s">
+      <c r="S21" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="2:19">
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
-      <c r="Q21" s="2"/>
-      <c r="R21" s="2"/>
-      <c r="S21" s="2"/>
     </row>
     <row r="22" spans="2:19">
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
-      <c r="P22" s="2"/>
-      <c r="Q22" s="2"/>
-      <c r="R22" s="2"/>
+      <c r="B22" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="1">
+        <v>82.679000000000002</v>
+      </c>
+      <c r="D22" s="1">
+        <v>89.275499999999994</v>
+      </c>
+      <c r="E22" s="1">
+        <v>91.245599999999996</v>
+      </c>
+      <c r="F22" s="1">
+        <v>83.225099999999998</v>
+      </c>
+      <c r="G22" s="1">
+        <v>84.73</v>
+      </c>
+      <c r="H22" s="1">
+        <v>112.809</v>
+      </c>
+      <c r="I22" s="1">
+        <v>113.81</v>
+      </c>
+      <c r="J22" s="1">
+        <v>113.301</v>
+      </c>
+      <c r="K22" s="1">
+        <v>124.33199999999999</v>
+      </c>
+      <c r="L22" s="1">
+        <v>117.312</v>
+      </c>
+      <c r="M22" s="1">
+        <v>98.2607</v>
+      </c>
+      <c r="N22" s="1">
+        <v>79.713499999999996</v>
+      </c>
+      <c r="O22" s="1">
+        <v>81.215199999999996</v>
+      </c>
+      <c r="P22" s="1">
+        <v>95.755099999999999</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>80.217600000000004</v>
+      </c>
+      <c r="R22" s="1">
+        <v>78.213399999999993</v>
+      </c>
       <c r="S22" s="2"/>
     </row>
     <row r="23" spans="2:19">
@@ -1896,15 +2157,34 @@
       <c r="R23" s="2"/>
       <c r="S23" s="2"/>
     </row>
+    <row r="24" spans="2:19">
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
+      <c r="S24" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1916,7 +2196,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>